<commit_message>
Fix small mistake in the sheets of Section 3.3
</commit_message>
<xml_diff>
--- a/chapter-3/section-3.3/sheets/canada.xlsx
+++ b/chapter-3/section-3.3/sheets/canada.xlsx
@@ -3691,8 +3691,8 @@
     </row>
     <row r="11">
       <c r="A11" s="12">
-        <f t="shared" ref="A11:A310" si="9">ROW()-9</f>
-        <v>2</v>
+        <f t="shared" ref="A11:A310" si="9">ROW()-10</f>
+        <v>1</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>14</v>
@@ -3723,7 +3723,7 @@
     <row r="12">
       <c r="A12" s="12">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>16</v>
@@ -3754,7 +3754,7 @@
     <row r="13">
       <c r="A13" s="12">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>18</v>
@@ -3785,7 +3785,7 @@
     <row r="14">
       <c r="A14" s="12">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>20</v>
@@ -3816,7 +3816,7 @@
     <row r="15">
       <c r="A15" s="12">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>22</v>
@@ -3847,7 +3847,7 @@
     <row r="16">
       <c r="A16" s="12">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>24</v>
@@ -3878,7 +3878,7 @@
     <row r="17">
       <c r="A17" s="12">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>26</v>
@@ -3909,7 +3909,7 @@
     <row r="18">
       <c r="A18" s="12">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>28</v>
@@ -3940,7 +3940,7 @@
     <row r="19">
       <c r="A19" s="12">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>30</v>
@@ -3971,7 +3971,7 @@
     <row r="20">
       <c r="A20" s="12">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>32</v>
@@ -4002,7 +4002,7 @@
     <row r="21">
       <c r="A21" s="12">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>34</v>
@@ -4033,7 +4033,7 @@
     <row r="22">
       <c r="A22" s="12">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>36</v>
@@ -4064,7 +4064,7 @@
     <row r="23">
       <c r="A23" s="12">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>38</v>
@@ -4095,7 +4095,7 @@
     <row r="24">
       <c r="A24" s="12">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>40</v>
@@ -4126,7 +4126,7 @@
     <row r="25">
       <c r="A25" s="12">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>42</v>
@@ -4157,7 +4157,7 @@
     <row r="26">
       <c r="A26" s="12">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>44</v>
@@ -4188,7 +4188,7 @@
     <row r="27">
       <c r="A27" s="12">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>46</v>
@@ -4219,7 +4219,7 @@
     <row r="28">
       <c r="A28" s="12">
         <f t="shared" si="9"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>48</v>
@@ -4250,7 +4250,7 @@
     <row r="29">
       <c r="A29" s="12">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>50</v>
@@ -4281,7 +4281,7 @@
     <row r="30">
       <c r="A30" s="12">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>52</v>
@@ -4312,7 +4312,7 @@
     <row r="31">
       <c r="A31" s="12">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>54</v>
@@ -4343,7 +4343,7 @@
     <row r="32">
       <c r="A32" s="12">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>56</v>
@@ -4374,7 +4374,7 @@
     <row r="33">
       <c r="A33" s="12">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>58</v>
@@ -4405,7 +4405,7 @@
     <row r="34">
       <c r="A34" s="12">
         <f t="shared" si="9"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>60</v>
@@ -4436,7 +4436,7 @@
     <row r="35">
       <c r="A35" s="12">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>62</v>
@@ -4467,7 +4467,7 @@
     <row r="36">
       <c r="A36" s="12">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>64</v>
@@ -4498,7 +4498,7 @@
     <row r="37">
       <c r="A37" s="12">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>66</v>
@@ -4529,7 +4529,7 @@
     <row r="38">
       <c r="A38" s="12">
         <f t="shared" si="9"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>68</v>
@@ -4560,7 +4560,7 @@
     <row r="39">
       <c r="A39" s="12">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>71</v>
@@ -4591,7 +4591,7 @@
     <row r="40">
       <c r="A40" s="12">
         <f t="shared" si="9"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>74</v>
@@ -4622,7 +4622,7 @@
     <row r="41">
       <c r="A41" s="12">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>77</v>
@@ -4653,7 +4653,7 @@
     <row r="42">
       <c r="A42" s="12">
         <f t="shared" si="9"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>80</v>
@@ -4684,7 +4684,7 @@
     <row r="43">
       <c r="A43" s="12">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>83</v>
@@ -4715,7 +4715,7 @@
     <row r="44">
       <c r="A44" s="12">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>86</v>
@@ -4746,7 +4746,7 @@
     <row r="45">
       <c r="A45" s="12">
         <f t="shared" si="9"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>89</v>
@@ -4777,7 +4777,7 @@
     <row r="46">
       <c r="A46" s="12">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>92</v>
@@ -4808,7 +4808,7 @@
     <row r="47">
       <c r="A47" s="12">
         <f t="shared" si="9"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>95</v>
@@ -4839,7 +4839,7 @@
     <row r="48">
       <c r="A48" s="12">
         <f t="shared" si="9"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>98</v>
@@ -4870,7 +4870,7 @@
     <row r="49">
       <c r="A49" s="12">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>101</v>
@@ -4901,7 +4901,7 @@
     <row r="50">
       <c r="A50" s="12">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>104</v>
@@ -4932,7 +4932,7 @@
     <row r="51">
       <c r="A51" s="12">
         <f t="shared" si="9"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>107</v>
@@ -4963,7 +4963,7 @@
     <row r="52">
       <c r="A52" s="12">
         <f t="shared" si="9"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>110</v>
@@ -4994,7 +4994,7 @@
     <row r="53">
       <c r="A53" s="12">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>113</v>
@@ -5025,7 +5025,7 @@
     <row r="54">
       <c r="A54" s="12">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>116</v>
@@ -5056,7 +5056,7 @@
     <row r="55">
       <c r="A55" s="12">
         <f t="shared" si="9"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>119</v>
@@ -5087,7 +5087,7 @@
     <row r="56">
       <c r="A56" s="12">
         <f t="shared" si="9"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>122</v>
@@ -5118,7 +5118,7 @@
     <row r="57">
       <c r="A57" s="12">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>125</v>
@@ -5149,7 +5149,7 @@
     <row r="58">
       <c r="A58" s="12">
         <f t="shared" si="9"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>128</v>
@@ -5180,7 +5180,7 @@
     <row r="59">
       <c r="A59" s="12">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>131</v>
@@ -5211,7 +5211,7 @@
     <row r="60">
       <c r="A60" s="12">
         <f t="shared" si="9"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>134</v>
@@ -5242,7 +5242,7 @@
     <row r="61">
       <c r="A61" s="12">
         <f t="shared" si="9"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>136</v>
@@ -5273,7 +5273,7 @@
     <row r="62">
       <c r="A62" s="12">
         <f t="shared" si="9"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>139</v>
@@ -5304,7 +5304,7 @@
     <row r="63">
       <c r="A63" s="12">
         <f t="shared" si="9"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>142</v>
@@ -5335,7 +5335,7 @@
     <row r="64">
       <c r="A64" s="12">
         <f t="shared" si="9"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>145</v>
@@ -5366,7 +5366,7 @@
     <row r="65">
       <c r="A65" s="12">
         <f t="shared" si="9"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>148</v>
@@ -5397,7 +5397,7 @@
     <row r="66">
       <c r="A66" s="12">
         <f t="shared" si="9"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>151</v>
@@ -5428,7 +5428,7 @@
     <row r="67">
       <c r="A67" s="12">
         <f t="shared" si="9"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>154</v>
@@ -5459,7 +5459,7 @@
     <row r="68">
       <c r="A68" s="12">
         <f t="shared" si="9"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>157</v>
@@ -5490,7 +5490,7 @@
     <row r="69">
       <c r="A69" s="12">
         <f t="shared" si="9"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>160</v>
@@ -5521,7 +5521,7 @@
     <row r="70">
       <c r="A70" s="12">
         <f t="shared" si="9"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>162</v>
@@ -5552,7 +5552,7 @@
     <row r="71">
       <c r="A71" s="12">
         <f t="shared" si="9"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>165</v>
@@ -5583,7 +5583,7 @@
     <row r="72">
       <c r="A72" s="12">
         <f t="shared" si="9"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>168</v>
@@ -5614,7 +5614,7 @@
     <row r="73">
       <c r="A73" s="12">
         <f t="shared" si="9"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>171</v>
@@ -5645,7 +5645,7 @@
     <row r="74">
       <c r="A74" s="12">
         <f t="shared" si="9"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>174</v>
@@ -5676,7 +5676,7 @@
     <row r="75">
       <c r="A75" s="12">
         <f t="shared" si="9"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>177</v>
@@ -5707,7 +5707,7 @@
     <row r="76">
       <c r="A76" s="12">
         <f t="shared" si="9"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>180</v>
@@ -5738,7 +5738,7 @@
     <row r="77">
       <c r="A77" s="12">
         <f t="shared" si="9"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>183</v>
@@ -5769,7 +5769,7 @@
     <row r="78">
       <c r="A78" s="12">
         <f t="shared" si="9"/>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>186</v>
@@ -5800,7 +5800,7 @@
     <row r="79">
       <c r="A79" s="12">
         <f t="shared" si="9"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>189</v>
@@ -5831,7 +5831,7 @@
     <row r="80">
       <c r="A80" s="12">
         <f t="shared" si="9"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>192</v>
@@ -5862,7 +5862,7 @@
     <row r="81">
       <c r="A81" s="12">
         <f t="shared" si="9"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>195</v>
@@ -5893,7 +5893,7 @@
     <row r="82">
       <c r="A82" s="12">
         <f t="shared" si="9"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>198</v>
@@ -5924,7 +5924,7 @@
     <row r="83">
       <c r="A83" s="12">
         <f t="shared" si="9"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>201</v>
@@ -5955,7 +5955,7 @@
     <row r="84">
       <c r="A84" s="12">
         <f t="shared" si="9"/>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>204</v>
@@ -5986,7 +5986,7 @@
     <row r="85">
       <c r="A85" s="12">
         <f t="shared" si="9"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>206</v>
@@ -6017,7 +6017,7 @@
     <row r="86">
       <c r="A86" s="12">
         <f t="shared" si="9"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>209</v>
@@ -6048,7 +6048,7 @@
     <row r="87">
       <c r="A87" s="12">
         <f t="shared" si="9"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>212</v>
@@ -6079,7 +6079,7 @@
     <row r="88">
       <c r="A88" s="12">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>215</v>
@@ -6110,7 +6110,7 @@
     <row r="89">
       <c r="A89" s="12">
         <f t="shared" si="9"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>218</v>
@@ -6141,7 +6141,7 @@
     <row r="90">
       <c r="A90" s="12">
         <f t="shared" si="9"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>221</v>
@@ -6172,7 +6172,7 @@
     <row r="91">
       <c r="A91" s="12">
         <f t="shared" si="9"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>224</v>
@@ -6203,7 +6203,7 @@
     <row r="92">
       <c r="A92" s="12">
         <f t="shared" si="9"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>227</v>
@@ -6234,7 +6234,7 @@
     <row r="93">
       <c r="A93" s="12">
         <f t="shared" si="9"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>230</v>
@@ -6265,7 +6265,7 @@
     <row r="94">
       <c r="A94" s="12">
         <f t="shared" si="9"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>233</v>
@@ -6296,7 +6296,7 @@
     <row r="95">
       <c r="A95" s="12">
         <f t="shared" si="9"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>236</v>
@@ -6327,7 +6327,7 @@
     <row r="96">
       <c r="A96" s="12">
         <f t="shared" si="9"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>239</v>
@@ -6358,7 +6358,7 @@
     <row r="97">
       <c r="A97" s="12">
         <f t="shared" si="9"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>241</v>
@@ -6389,7 +6389,7 @@
     <row r="98">
       <c r="A98" s="12">
         <f t="shared" si="9"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B98" s="13" t="s">
         <v>244</v>
@@ -6420,7 +6420,7 @@
     <row r="99">
       <c r="A99" s="12">
         <f t="shared" si="9"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B99" s="13" t="s">
         <v>247</v>
@@ -6451,7 +6451,7 @@
     <row r="100">
       <c r="A100" s="12">
         <f t="shared" si="9"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>250</v>
@@ -6482,7 +6482,7 @@
     <row r="101">
       <c r="A101" s="12">
         <f t="shared" si="9"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>253</v>
@@ -6513,7 +6513,7 @@
     <row r="102">
       <c r="A102" s="12">
         <f t="shared" si="9"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>256</v>
@@ -6544,7 +6544,7 @@
     <row r="103">
       <c r="A103" s="12">
         <f t="shared" si="9"/>
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>259</v>
@@ -6575,7 +6575,7 @@
     <row r="104">
       <c r="A104" s="12">
         <f t="shared" si="9"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B104" s="13" t="s">
         <v>262</v>
@@ -6606,7 +6606,7 @@
     <row r="105">
       <c r="A105" s="12">
         <f t="shared" si="9"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B105" s="13" t="s">
         <v>265</v>
@@ -6637,7 +6637,7 @@
     <row r="106">
       <c r="A106" s="12">
         <f t="shared" si="9"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>268</v>
@@ -6668,7 +6668,7 @@
     <row r="107">
       <c r="A107" s="12">
         <f t="shared" si="9"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" s="13" t="s">
         <v>271</v>
@@ -6699,7 +6699,7 @@
     <row r="108">
       <c r="A108" s="12">
         <f t="shared" si="9"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B108" s="13" t="s">
         <v>274</v>
@@ -6730,7 +6730,7 @@
     <row r="109">
       <c r="A109" s="12">
         <f t="shared" si="9"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B109" s="13" t="s">
         <v>277</v>
@@ -6761,7 +6761,7 @@
     <row r="110">
       <c r="A110" s="12">
         <f t="shared" si="9"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B110" s="13" t="s">
         <v>280</v>
@@ -6792,7 +6792,7 @@
     <row r="111">
       <c r="A111" s="12">
         <f t="shared" si="9"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>283</v>
@@ -6823,7 +6823,7 @@
     <row r="112">
       <c r="A112" s="12">
         <f t="shared" si="9"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>286</v>
@@ -6854,7 +6854,7 @@
     <row r="113">
       <c r="A113" s="12">
         <f t="shared" si="9"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113" s="13" t="s">
         <v>289</v>
@@ -6885,7 +6885,7 @@
     <row r="114">
       <c r="A114" s="12">
         <f t="shared" si="9"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B114" s="13" t="s">
         <v>292</v>
@@ -6916,7 +6916,7 @@
     <row r="115">
       <c r="A115" s="12">
         <f t="shared" si="9"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>295</v>
@@ -6947,7 +6947,7 @@
     <row r="116">
       <c r="A116" s="12">
         <f t="shared" si="9"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B116" s="13" t="s">
         <v>298</v>
@@ -6978,7 +6978,7 @@
     <row r="117">
       <c r="A117" s="12">
         <f t="shared" si="9"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B117" s="13" t="s">
         <v>301</v>
@@ -7009,7 +7009,7 @@
     <row r="118">
       <c r="A118" s="12">
         <f t="shared" si="9"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>304</v>
@@ -7040,7 +7040,7 @@
     <row r="119">
       <c r="A119" s="12">
         <f t="shared" si="9"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>306</v>
@@ -7071,7 +7071,7 @@
     <row r="120">
       <c r="A120" s="12">
         <f t="shared" si="9"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B120" s="13" t="s">
         <v>309</v>
@@ -7102,7 +7102,7 @@
     <row r="121">
       <c r="A121" s="12">
         <f t="shared" si="9"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B121" s="13" t="s">
         <v>312</v>
@@ -7133,7 +7133,7 @@
     <row r="122">
       <c r="A122" s="12">
         <f t="shared" si="9"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B122" s="13" t="s">
         <v>315</v>
@@ -7164,7 +7164,7 @@
     <row r="123">
       <c r="A123" s="12">
         <f t="shared" si="9"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>318</v>
@@ -7195,7 +7195,7 @@
     <row r="124">
       <c r="A124" s="12">
         <f t="shared" si="9"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>321</v>
@@ -7226,7 +7226,7 @@
     <row r="125">
       <c r="A125" s="12">
         <f t="shared" si="9"/>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>323</v>
@@ -7257,7 +7257,7 @@
     <row r="126">
       <c r="A126" s="12">
         <f t="shared" si="9"/>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B126" s="13" t="s">
         <v>326</v>
@@ -7288,7 +7288,7 @@
     <row r="127">
       <c r="A127" s="12">
         <f t="shared" si="9"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B127" s="13" t="s">
         <v>329</v>
@@ -7319,7 +7319,7 @@
     <row r="128">
       <c r="A128" s="12">
         <f t="shared" si="9"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B128" s="13" t="s">
         <v>332</v>
@@ -7350,7 +7350,7 @@
     <row r="129">
       <c r="A129" s="12">
         <f t="shared" si="9"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B129" s="13" t="s">
         <v>335</v>
@@ -7381,7 +7381,7 @@
     <row r="130">
       <c r="A130" s="12">
         <f t="shared" si="9"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B130" s="13" t="s">
         <v>338</v>
@@ -7412,7 +7412,7 @@
     <row r="131">
       <c r="A131" s="12">
         <f t="shared" si="9"/>
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B131" s="13" t="s">
         <v>340</v>
@@ -7443,7 +7443,7 @@
     <row r="132">
       <c r="A132" s="12">
         <f t="shared" si="9"/>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B132" s="13" t="s">
         <v>343</v>
@@ -7474,7 +7474,7 @@
     <row r="133">
       <c r="A133" s="12">
         <f t="shared" si="9"/>
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B133" s="13" t="s">
         <v>346</v>
@@ -7505,7 +7505,7 @@
     <row r="134">
       <c r="A134" s="12">
         <f t="shared" si="9"/>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B134" s="13" t="s">
         <v>349</v>
@@ -7536,7 +7536,7 @@
     <row r="135">
       <c r="A135" s="12">
         <f t="shared" si="9"/>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B135" s="13" t="s">
         <v>352</v>
@@ -7567,7 +7567,7 @@
     <row r="136">
       <c r="A136" s="12">
         <f t="shared" si="9"/>
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B136" s="13" t="s">
         <v>355</v>
@@ -7598,7 +7598,7 @@
     <row r="137">
       <c r="A137" s="12">
         <f t="shared" si="9"/>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B137" s="13" t="s">
         <v>358</v>
@@ -7629,7 +7629,7 @@
     <row r="138">
       <c r="A138" s="12">
         <f t="shared" si="9"/>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B138" s="13" t="s">
         <v>361</v>
@@ -7660,7 +7660,7 @@
     <row r="139">
       <c r="A139" s="12">
         <f t="shared" si="9"/>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B139" s="13" t="s">
         <v>364</v>
@@ -7691,7 +7691,7 @@
     <row r="140">
       <c r="A140" s="12">
         <f t="shared" si="9"/>
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B140" s="13" t="s">
         <v>367</v>
@@ -7722,7 +7722,7 @@
     <row r="141">
       <c r="A141" s="12">
         <f t="shared" si="9"/>
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B141" s="13" t="s">
         <v>370</v>
@@ -7753,7 +7753,7 @@
     <row r="142">
       <c r="A142" s="12">
         <f t="shared" si="9"/>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B142" s="13" t="s">
         <v>373</v>
@@ -7784,7 +7784,7 @@
     <row r="143">
       <c r="A143" s="12">
         <f t="shared" si="9"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B143" s="13" t="s">
         <v>376</v>
@@ -7815,7 +7815,7 @@
     <row r="144">
       <c r="A144" s="12">
         <f t="shared" si="9"/>
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B144" s="13" t="s">
         <v>378</v>
@@ -7846,7 +7846,7 @@
     <row r="145">
       <c r="A145" s="12">
         <f t="shared" si="9"/>
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B145" s="13" t="s">
         <v>381</v>
@@ -7877,7 +7877,7 @@
     <row r="146">
       <c r="A146" s="12">
         <f t="shared" si="9"/>
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B146" s="13" t="s">
         <v>384</v>
@@ -7908,7 +7908,7 @@
     <row r="147">
       <c r="A147" s="12">
         <f t="shared" si="9"/>
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B147" s="13" t="s">
         <v>387</v>
@@ -7939,7 +7939,7 @@
     <row r="148">
       <c r="A148" s="12">
         <f t="shared" si="9"/>
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B148" s="13" t="s">
         <v>390</v>
@@ -7970,7 +7970,7 @@
     <row r="149">
       <c r="A149" s="12">
         <f t="shared" si="9"/>
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B149" s="13" t="s">
         <v>393</v>
@@ -8001,7 +8001,7 @@
     <row r="150">
       <c r="A150" s="12">
         <f t="shared" si="9"/>
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B150" s="13" t="s">
         <v>396</v>
@@ -8032,7 +8032,7 @@
     <row r="151">
       <c r="A151" s="12">
         <f t="shared" si="9"/>
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B151" s="13" t="s">
         <v>399</v>
@@ -8063,7 +8063,7 @@
     <row r="152">
       <c r="A152" s="12">
         <f t="shared" si="9"/>
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B152" s="13" t="s">
         <v>402</v>
@@ -8094,7 +8094,7 @@
     <row r="153">
       <c r="A153" s="12">
         <f t="shared" si="9"/>
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B153" s="13" t="s">
         <v>405</v>
@@ -8125,7 +8125,7 @@
     <row r="154">
       <c r="A154" s="12">
         <f t="shared" si="9"/>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B154" s="13" t="s">
         <v>408</v>
@@ -8156,7 +8156,7 @@
     <row r="155">
       <c r="A155" s="12">
         <f t="shared" si="9"/>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B155" s="13" t="s">
         <v>411</v>
@@ -8187,7 +8187,7 @@
     <row r="156">
       <c r="A156" s="12">
         <f t="shared" si="9"/>
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B156" s="13" t="s">
         <v>414</v>
@@ -8218,7 +8218,7 @@
     <row r="157">
       <c r="A157" s="12">
         <f t="shared" si="9"/>
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B157" s="13" t="s">
         <v>417</v>
@@ -8249,7 +8249,7 @@
     <row r="158">
       <c r="A158" s="12">
         <f t="shared" si="9"/>
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B158" s="13" t="s">
         <v>420</v>
@@ -8280,7 +8280,7 @@
     <row r="159">
       <c r="A159" s="12">
         <f t="shared" si="9"/>
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B159" s="13" t="s">
         <v>423</v>
@@ -8311,7 +8311,7 @@
     <row r="160">
       <c r="A160" s="12">
         <f t="shared" si="9"/>
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B160" s="13" t="s">
         <v>426</v>
@@ -8342,7 +8342,7 @@
     <row r="161">
       <c r="A161" s="12">
         <f t="shared" si="9"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B161" s="13" t="s">
         <v>429</v>
@@ -8373,7 +8373,7 @@
     <row r="162">
       <c r="A162" s="12">
         <f t="shared" si="9"/>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B162" s="13" t="s">
         <v>432</v>
@@ -8404,7 +8404,7 @@
     <row r="163">
       <c r="A163" s="12">
         <f t="shared" si="9"/>
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B163" s="13" t="s">
         <v>435</v>
@@ -8435,7 +8435,7 @@
     <row r="164">
       <c r="A164" s="12">
         <f t="shared" si="9"/>
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B164" s="13" t="s">
         <v>438</v>
@@ -8466,7 +8466,7 @@
     <row r="165">
       <c r="A165" s="12">
         <f t="shared" si="9"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B165" s="13" t="s">
         <v>441</v>
@@ -8497,7 +8497,7 @@
     <row r="166">
       <c r="A166" s="12">
         <f t="shared" si="9"/>
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B166" s="13" t="s">
         <v>444</v>
@@ -8528,7 +8528,7 @@
     <row r="167">
       <c r="A167" s="12">
         <f t="shared" si="9"/>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B167" s="13" t="s">
         <v>447</v>
@@ -8556,7 +8556,7 @@
     <row r="168">
       <c r="A168" s="12">
         <f t="shared" si="9"/>
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B168" s="13" t="s">
         <v>449</v>
@@ -8584,7 +8584,7 @@
     <row r="169">
       <c r="A169" s="12">
         <f t="shared" si="9"/>
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B169" s="13" t="s">
         <v>451</v>
@@ -8612,7 +8612,7 @@
     <row r="170">
       <c r="A170" s="12">
         <f t="shared" si="9"/>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B170" s="13" t="s">
         <v>453</v>
@@ -8640,7 +8640,7 @@
     <row r="171">
       <c r="A171" s="12">
         <f t="shared" si="9"/>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>455</v>
@@ -8668,7 +8668,7 @@
     <row r="172">
       <c r="A172" s="12">
         <f t="shared" si="9"/>
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B172" s="13" t="s">
         <v>457</v>
@@ -8696,7 +8696,7 @@
     <row r="173">
       <c r="A173" s="12">
         <f t="shared" si="9"/>
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B173" s="13" t="s">
         <v>459</v>
@@ -8724,7 +8724,7 @@
     <row r="174">
       <c r="A174" s="12">
         <f t="shared" si="9"/>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B174" s="13" t="s">
         <v>461</v>
@@ -8752,7 +8752,7 @@
     <row r="175">
       <c r="A175" s="12">
         <f t="shared" si="9"/>
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B175" s="13" t="s">
         <v>463</v>
@@ -8780,7 +8780,7 @@
     <row r="176">
       <c r="A176" s="12">
         <f t="shared" si="9"/>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B176" s="13" t="s">
         <v>465</v>
@@ -8808,7 +8808,7 @@
     <row r="177">
       <c r="A177" s="12">
         <f t="shared" si="9"/>
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B177" s="13" t="s">
         <v>467</v>
@@ -8836,7 +8836,7 @@
     <row r="178">
       <c r="A178" s="12">
         <f t="shared" si="9"/>
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B178" s="13" t="s">
         <v>469</v>
@@ -8864,7 +8864,7 @@
     <row r="179">
       <c r="A179" s="12">
         <f t="shared" si="9"/>
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B179" s="13" t="s">
         <v>471</v>
@@ -8892,7 +8892,7 @@
     <row r="180">
       <c r="A180" s="12">
         <f t="shared" si="9"/>
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B180" s="13" t="s">
         <v>473</v>
@@ -8920,7 +8920,7 @@
     <row r="181">
       <c r="A181" s="12">
         <f t="shared" si="9"/>
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B181" s="13" t="s">
         <v>475</v>
@@ -8948,7 +8948,7 @@
     <row r="182">
       <c r="A182" s="12">
         <f t="shared" si="9"/>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B182" s="13" t="s">
         <v>477</v>
@@ -8976,7 +8976,7 @@
     <row r="183">
       <c r="A183" s="12">
         <f t="shared" si="9"/>
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B183" s="13" t="s">
         <v>479</v>
@@ -9004,7 +9004,7 @@
     <row r="184">
       <c r="A184" s="12">
         <f t="shared" si="9"/>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B184" s="13" t="s">
         <v>481</v>
@@ -9032,7 +9032,7 @@
     <row r="185">
       <c r="A185" s="12">
         <f t="shared" si="9"/>
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B185" s="13" t="s">
         <v>483</v>
@@ -9060,7 +9060,7 @@
     <row r="186">
       <c r="A186" s="12">
         <f t="shared" si="9"/>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B186" s="13" t="s">
         <v>485</v>
@@ -9088,7 +9088,7 @@
     <row r="187">
       <c r="A187" s="12">
         <f t="shared" si="9"/>
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B187" s="13" t="s">
         <v>487</v>
@@ -9116,7 +9116,7 @@
     <row r="188">
       <c r="A188" s="12">
         <f t="shared" si="9"/>
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B188" s="13" t="s">
         <v>489</v>
@@ -9144,7 +9144,7 @@
     <row r="189">
       <c r="A189" s="12">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B189" s="13" t="s">
         <v>491</v>
@@ -9172,7 +9172,7 @@
     <row r="190">
       <c r="A190" s="12">
         <f t="shared" si="9"/>
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B190" s="13" t="s">
         <v>493</v>
@@ -9200,7 +9200,7 @@
     <row r="191">
       <c r="A191" s="12">
         <f t="shared" si="9"/>
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B191" s="13" t="s">
         <v>495</v>
@@ -9228,7 +9228,7 @@
     <row r="192">
       <c r="A192" s="12">
         <f t="shared" si="9"/>
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B192" s="13" t="s">
         <v>497</v>
@@ -9256,7 +9256,7 @@
     <row r="193">
       <c r="A193" s="12">
         <f t="shared" si="9"/>
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B193" s="13" t="s">
         <v>499</v>
@@ -9284,7 +9284,7 @@
     <row r="194">
       <c r="A194" s="12">
         <f t="shared" si="9"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B194" s="13" t="s">
         <v>501</v>
@@ -9312,7 +9312,7 @@
     <row r="195">
       <c r="A195" s="12">
         <f t="shared" si="9"/>
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B195" s="13" t="s">
         <v>503</v>
@@ -9340,7 +9340,7 @@
     <row r="196">
       <c r="A196" s="12">
         <f t="shared" si="9"/>
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B196" s="13" t="s">
         <v>505</v>
@@ -9368,7 +9368,7 @@
     <row r="197">
       <c r="A197" s="12">
         <f t="shared" si="9"/>
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B197" s="13" t="s">
         <v>507</v>
@@ -9396,7 +9396,7 @@
     <row r="198">
       <c r="A198" s="12">
         <f t="shared" si="9"/>
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B198" s="13" t="s">
         <v>509</v>
@@ -9424,7 +9424,7 @@
     <row r="199">
       <c r="A199" s="12">
         <f t="shared" si="9"/>
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B199" s="13" t="s">
         <v>511</v>
@@ -9452,7 +9452,7 @@
     <row r="200">
       <c r="A200" s="12">
         <f t="shared" si="9"/>
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B200" s="13" t="s">
         <v>513</v>
@@ -9480,7 +9480,7 @@
     <row r="201">
       <c r="A201" s="12">
         <f t="shared" si="9"/>
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B201" s="13" t="s">
         <v>515</v>
@@ -9508,7 +9508,7 @@
     <row r="202">
       <c r="A202" s="12">
         <f t="shared" si="9"/>
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B202" s="13" t="s">
         <v>517</v>
@@ -9536,7 +9536,7 @@
     <row r="203">
       <c r="A203" s="12">
         <f t="shared" si="9"/>
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B203" s="13" t="s">
         <v>519</v>
@@ -9564,7 +9564,7 @@
     <row r="204">
       <c r="A204" s="12">
         <f t="shared" si="9"/>
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B204" s="13" t="s">
         <v>521</v>
@@ -9592,7 +9592,7 @@
     <row r="205">
       <c r="A205" s="12">
         <f t="shared" si="9"/>
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B205" s="13" t="s">
         <v>523</v>
@@ -9620,7 +9620,7 @@
     <row r="206">
       <c r="A206" s="12">
         <f t="shared" si="9"/>
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B206" s="13" t="s">
         <v>525</v>
@@ -9648,7 +9648,7 @@
     <row r="207">
       <c r="A207" s="12">
         <f t="shared" si="9"/>
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B207" s="13" t="s">
         <v>527</v>
@@ -9676,7 +9676,7 @@
     <row r="208">
       <c r="A208" s="12">
         <f t="shared" si="9"/>
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B208" s="13" t="s">
         <v>529</v>
@@ -9704,7 +9704,7 @@
     <row r="209">
       <c r="A209" s="12">
         <f t="shared" si="9"/>
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B209" s="13" t="s">
         <v>531</v>
@@ -9732,7 +9732,7 @@
     <row r="210">
       <c r="A210" s="12">
         <f t="shared" si="9"/>
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B210" s="13" t="s">
         <v>533</v>
@@ -9760,7 +9760,7 @@
     <row r="211">
       <c r="A211" s="12">
         <f t="shared" si="9"/>
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B211" s="13" t="s">
         <v>535</v>
@@ -9788,7 +9788,7 @@
     <row r="212">
       <c r="A212" s="12">
         <f t="shared" si="9"/>
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B212" s="13" t="s">
         <v>537</v>
@@ -9816,7 +9816,7 @@
     <row r="213">
       <c r="A213" s="12">
         <f t="shared" si="9"/>
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B213" s="13" t="s">
         <v>539</v>
@@ -9844,7 +9844,7 @@
     <row r="214">
       <c r="A214" s="12">
         <f t="shared" si="9"/>
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B214" s="13" t="s">
         <v>541</v>
@@ -9872,7 +9872,7 @@
     <row r="215">
       <c r="A215" s="12">
         <f t="shared" si="9"/>
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B215" s="13" t="s">
         <v>543</v>
@@ -9900,7 +9900,7 @@
     <row r="216">
       <c r="A216" s="12">
         <f t="shared" si="9"/>
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B216" s="13" t="s">
         <v>545</v>
@@ -9928,7 +9928,7 @@
     <row r="217">
       <c r="A217" s="12">
         <f t="shared" si="9"/>
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B217" s="13" t="s">
         <v>547</v>
@@ -9956,7 +9956,7 @@
     <row r="218">
       <c r="A218" s="12">
         <f t="shared" si="9"/>
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>549</v>
@@ -9984,7 +9984,7 @@
     <row r="219">
       <c r="A219" s="12">
         <f t="shared" si="9"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B219" s="13" t="s">
         <v>551</v>
@@ -10012,7 +10012,7 @@
     <row r="220">
       <c r="A220" s="12">
         <f t="shared" si="9"/>
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B220" s="13" t="s">
         <v>553</v>
@@ -10040,7 +10040,7 @@
     <row r="221">
       <c r="A221" s="12">
         <f t="shared" si="9"/>
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B221" s="13" t="s">
         <v>555</v>
@@ -10068,7 +10068,7 @@
     <row r="222">
       <c r="A222" s="12">
         <f t="shared" si="9"/>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>557</v>
@@ -10096,7 +10096,7 @@
     <row r="223">
       <c r="A223" s="12">
         <f t="shared" si="9"/>
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B223" s="13" t="s">
         <v>559</v>
@@ -10124,7 +10124,7 @@
     <row r="224">
       <c r="A224" s="12">
         <f t="shared" si="9"/>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B224" s="13" t="s">
         <v>561</v>
@@ -10152,7 +10152,7 @@
     <row r="225">
       <c r="A225" s="12">
         <f t="shared" si="9"/>
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B225" s="13" t="s">
         <v>563</v>
@@ -10180,7 +10180,7 @@
     <row r="226">
       <c r="A226" s="12">
         <f t="shared" si="9"/>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B226" s="13" t="s">
         <v>565</v>
@@ -10208,7 +10208,7 @@
     <row r="227">
       <c r="A227" s="12">
         <f t="shared" si="9"/>
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B227" s="13" t="s">
         <v>567</v>
@@ -10236,7 +10236,7 @@
     <row r="228">
       <c r="A228" s="12">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B228" s="13" t="s">
         <v>569</v>
@@ -10264,7 +10264,7 @@
     <row r="229">
       <c r="A229" s="12">
         <f t="shared" si="9"/>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B229" s="13" t="s">
         <v>571</v>
@@ -10292,7 +10292,7 @@
     <row r="230">
       <c r="A230" s="12">
         <f t="shared" si="9"/>
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B230" s="13" t="s">
         <v>573</v>
@@ -10320,7 +10320,7 @@
     <row r="231">
       <c r="A231" s="12">
         <f t="shared" si="9"/>
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B231" s="13" t="s">
         <v>575</v>
@@ -10348,7 +10348,7 @@
     <row r="232">
       <c r="A232" s="12">
         <f t="shared" si="9"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B232" s="13" t="s">
         <v>577</v>
@@ -10376,7 +10376,7 @@
     <row r="233">
       <c r="A233" s="12">
         <f t="shared" si="9"/>
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B233" s="13" t="s">
         <v>579</v>
@@ -10404,7 +10404,7 @@
     <row r="234">
       <c r="A234" s="12">
         <f t="shared" si="9"/>
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B234" s="13" t="s">
         <v>581</v>
@@ -10432,7 +10432,7 @@
     <row r="235">
       <c r="A235" s="12">
         <f t="shared" si="9"/>
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B235" s="13" t="s">
         <v>583</v>
@@ -10460,7 +10460,7 @@
     <row r="236">
       <c r="A236" s="12">
         <f t="shared" si="9"/>
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B236" s="13" t="s">
         <v>272</v>
@@ -10488,7 +10488,7 @@
     <row r="237">
       <c r="A237" s="12">
         <f t="shared" si="9"/>
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B237" s="13" t="s">
         <v>269</v>
@@ -10516,7 +10516,7 @@
     <row r="238">
       <c r="A238" s="12">
         <f t="shared" si="9"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B238" s="13" t="s">
         <v>184</v>
@@ -10544,7 +10544,7 @@
     <row r="239">
       <c r="A239" s="12">
         <f t="shared" si="9"/>
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B239" s="13" t="s">
         <v>222</v>
@@ -10572,7 +10572,7 @@
     <row r="240">
       <c r="A240" s="12">
         <f t="shared" si="9"/>
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B240" s="13" t="s">
         <v>81</v>
@@ -10600,7 +10600,7 @@
     <row r="241">
       <c r="A241" s="12">
         <f t="shared" si="9"/>
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B241" s="13" t="s">
         <v>190</v>
@@ -10628,7 +10628,7 @@
     <row r="242">
       <c r="A242" s="12">
         <f t="shared" si="9"/>
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B242" s="13" t="s">
         <v>591</v>
@@ -10656,7 +10656,7 @@
     <row r="243">
       <c r="A243" s="12">
         <f t="shared" si="9"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B243" s="13" t="s">
         <v>593</v>
@@ -10684,7 +10684,7 @@
     <row r="244">
       <c r="A244" s="12">
         <f t="shared" si="9"/>
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B244" s="13" t="s">
         <v>353</v>
@@ -10712,7 +10712,7 @@
     <row r="245">
       <c r="A245" s="12">
         <f t="shared" si="9"/>
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B245" s="13" t="s">
         <v>362</v>
@@ -10740,7 +10740,7 @@
     <row r="246">
       <c r="A246" s="12">
         <f t="shared" si="9"/>
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B246" s="13" t="s">
         <v>597</v>
@@ -10768,7 +10768,7 @@
     <row r="247">
       <c r="A247" s="12">
         <f t="shared" si="9"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B247" s="13" t="s">
         <v>599</v>
@@ -10796,7 +10796,7 @@
     <row r="248">
       <c r="A248" s="12">
         <f t="shared" si="9"/>
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B248" s="13" t="s">
         <v>260</v>
@@ -10824,7 +10824,7 @@
     <row r="249">
       <c r="A249" s="12">
         <f t="shared" si="9"/>
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B249" s="13" t="s">
         <v>319</v>
@@ -10852,7 +10852,7 @@
     <row r="250">
       <c r="A250" s="12">
         <f t="shared" si="9"/>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B250" s="13" t="s">
         <v>324</v>
@@ -10880,7 +10880,7 @@
     <row r="251">
       <c r="A251" s="12">
         <f t="shared" si="9"/>
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B251" s="13" t="s">
         <v>604</v>
@@ -10908,7 +10908,7 @@
     <row r="252">
       <c r="A252" s="12">
         <f t="shared" si="9"/>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B252" s="13" t="s">
         <v>606</v>
@@ -10936,7 +10936,7 @@
     <row r="253">
       <c r="A253" s="12">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B253" s="13" t="s">
         <v>608</v>
@@ -10964,7 +10964,7 @@
     <row r="254">
       <c r="A254" s="12">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B254" s="13" t="s">
         <v>610</v>
@@ -10992,7 +10992,7 @@
     <row r="255">
       <c r="A255" s="12">
         <f t="shared" si="9"/>
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B255" s="13" t="s">
         <v>612</v>
@@ -11020,7 +11020,7 @@
     <row r="256">
       <c r="A256" s="12">
         <f t="shared" si="9"/>
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B256" s="13" t="s">
         <v>614</v>
@@ -11048,7 +11048,7 @@
     <row r="257">
       <c r="A257" s="12">
         <f t="shared" si="9"/>
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B257" s="13" t="s">
         <v>616</v>
@@ -11076,7 +11076,7 @@
     <row r="258">
       <c r="A258" s="12">
         <f t="shared" si="9"/>
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B258" s="13" t="s">
         <v>618</v>
@@ -11104,7 +11104,7 @@
     <row r="259">
       <c r="A259" s="12">
         <f t="shared" si="9"/>
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B259" s="13" t="s">
         <v>347</v>
@@ -11132,7 +11132,7 @@
     <row r="260">
       <c r="A260" s="12">
         <f t="shared" si="9"/>
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B260" s="13" t="s">
         <v>621</v>
@@ -11160,7 +11160,7 @@
     <row r="261">
       <c r="A261" s="12">
         <f t="shared" si="9"/>
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B261" s="13" t="s">
         <v>623</v>
@@ -11188,7 +11188,7 @@
     <row r="262">
       <c r="A262" s="12">
         <f t="shared" si="9"/>
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B262" s="13" t="s">
         <v>625</v>
@@ -11216,7 +11216,7 @@
     <row r="263">
       <c r="A263" s="12">
         <f t="shared" si="9"/>
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B263" s="13" t="s">
         <v>627</v>
@@ -11244,7 +11244,7 @@
     <row r="264">
       <c r="A264" s="12">
         <f t="shared" si="9"/>
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B264" s="13" t="s">
         <v>629</v>
@@ -11272,7 +11272,7 @@
     <row r="265">
       <c r="A265" s="12">
         <f t="shared" si="9"/>
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B265" s="13" t="s">
         <v>631</v>
@@ -11300,7 +11300,7 @@
     <row r="266">
       <c r="A266" s="12">
         <f t="shared" si="9"/>
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B266" s="13" t="s">
         <v>633</v>
@@ -11328,7 +11328,7 @@
     <row r="267">
       <c r="A267" s="12">
         <f t="shared" si="9"/>
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B267" s="13" t="s">
         <v>635</v>
@@ -11356,7 +11356,7 @@
     <row r="268">
       <c r="A268" s="12">
         <f t="shared" si="9"/>
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B268" s="13" t="s">
         <v>637</v>
@@ -11384,7 +11384,7 @@
     <row r="269">
       <c r="A269" s="12">
         <f t="shared" si="9"/>
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B269" s="13" t="s">
         <v>639</v>
@@ -11412,7 +11412,7 @@
     <row r="270">
       <c r="A270" s="12">
         <f t="shared" si="9"/>
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B270" s="13" t="s">
         <v>641</v>
@@ -11440,7 +11440,7 @@
     <row r="271">
       <c r="A271" s="12">
         <f t="shared" si="9"/>
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B271" s="13" t="s">
         <v>169</v>
@@ -11468,7 +11468,7 @@
     <row r="272">
       <c r="A272" s="12">
         <f t="shared" si="9"/>
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B272" s="13" t="s">
         <v>210</v>
@@ -11496,7 +11496,7 @@
     <row r="273">
       <c r="A273" s="12">
         <f t="shared" si="9"/>
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B273" s="13" t="s">
         <v>251</v>
@@ -11524,7 +11524,7 @@
     <row r="274">
       <c r="A274" s="12">
         <f t="shared" si="9"/>
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B274" s="13" t="s">
         <v>646</v>
@@ -11552,7 +11552,7 @@
     <row r="275">
       <c r="A275" s="12">
         <f t="shared" si="9"/>
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B275" s="13" t="s">
         <v>350</v>
@@ -11580,7 +11580,7 @@
     <row r="276">
       <c r="A276" s="12">
         <f t="shared" si="9"/>
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B276" s="13" t="s">
         <v>649</v>
@@ -11608,7 +11608,7 @@
     <row r="277">
       <c r="A277" s="12">
         <f t="shared" si="9"/>
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B277" s="13" t="s">
         <v>651</v>
@@ -11636,7 +11636,7 @@
     <row r="278">
       <c r="A278" s="12">
         <f t="shared" si="9"/>
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B278" s="13" t="s">
         <v>653</v>
@@ -11664,7 +11664,7 @@
     <row r="279">
       <c r="A279" s="12">
         <f t="shared" si="9"/>
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B279" s="13" t="s">
         <v>655</v>
@@ -11692,7 +11692,7 @@
     <row r="280">
       <c r="A280" s="12">
         <f t="shared" si="9"/>
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B280" s="13" t="s">
         <v>657</v>
@@ -11720,7 +11720,7 @@
     <row r="281">
       <c r="A281" s="12">
         <f t="shared" si="9"/>
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B281" s="13" t="s">
         <v>659</v>
@@ -11748,7 +11748,7 @@
     <row r="282">
       <c r="A282" s="12">
         <f t="shared" si="9"/>
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B282" s="13" t="s">
         <v>661</v>
@@ -11776,7 +11776,7 @@
     <row r="283">
       <c r="A283" s="12">
         <f t="shared" si="9"/>
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B283" s="13" t="s">
         <v>663</v>
@@ -11804,7 +11804,7 @@
     <row r="284">
       <c r="A284" s="12">
         <f t="shared" si="9"/>
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B284" s="13" t="s">
         <v>665</v>
@@ -11832,7 +11832,7 @@
     <row r="285">
       <c r="A285" s="12">
         <f t="shared" si="9"/>
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B285" s="13" t="s">
         <v>667</v>
@@ -11860,7 +11860,7 @@
     <row r="286">
       <c r="A286" s="12">
         <f t="shared" si="9"/>
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B286" s="13" t="s">
         <v>669</v>
@@ -11888,7 +11888,7 @@
     <row r="287">
       <c r="A287" s="12">
         <f t="shared" si="9"/>
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B287" s="13" t="s">
         <v>671</v>
@@ -11916,7 +11916,7 @@
     <row r="288">
       <c r="A288" s="12">
         <f t="shared" si="9"/>
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B288" s="13" t="s">
         <v>307</v>
@@ -11944,7 +11944,7 @@
     <row r="289">
       <c r="A289" s="12">
         <f t="shared" si="9"/>
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B289" s="13" t="s">
         <v>674</v>
@@ -11972,7 +11972,7 @@
     <row r="290">
       <c r="A290" s="12">
         <f t="shared" si="9"/>
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B290" s="13" t="s">
         <v>676</v>
@@ -12000,7 +12000,7 @@
     <row r="291">
       <c r="A291" s="12">
         <f t="shared" si="9"/>
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B291" s="13" t="s">
         <v>678</v>
@@ -12028,7 +12028,7 @@
     <row r="292">
       <c r="A292" s="12">
         <f t="shared" si="9"/>
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B292" s="13" t="s">
         <v>680</v>
@@ -12056,7 +12056,7 @@
     <row r="293">
       <c r="A293" s="12">
         <f t="shared" si="9"/>
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B293" s="13" t="s">
         <v>682</v>
@@ -12084,7 +12084,7 @@
     <row r="294">
       <c r="A294" s="12">
         <f t="shared" si="9"/>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B294" s="13" t="s">
         <v>684</v>
@@ -12112,7 +12112,7 @@
     <row r="295">
       <c r="A295" s="12">
         <f t="shared" si="9"/>
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B295" s="13" t="s">
         <v>686</v>
@@ -12140,7 +12140,7 @@
     <row r="296">
       <c r="A296" s="12">
         <f t="shared" si="9"/>
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B296" s="13" t="s">
         <v>688</v>
@@ -12168,7 +12168,7 @@
     <row r="297">
       <c r="A297" s="12">
         <f t="shared" si="9"/>
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B297" s="13" t="s">
         <v>690</v>
@@ -12196,7 +12196,7 @@
     <row r="298">
       <c r="A298" s="12">
         <f t="shared" si="9"/>
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B298" s="13" t="s">
         <v>158</v>
@@ -12224,7 +12224,7 @@
     <row r="299">
       <c r="A299" s="12">
         <f t="shared" si="9"/>
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B299" s="13" t="s">
         <v>75</v>
@@ -12252,7 +12252,7 @@
     <row r="300">
       <c r="A300" s="12">
         <f t="shared" si="9"/>
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B300" s="13" t="s">
         <v>694</v>
@@ -12280,7 +12280,7 @@
     <row r="301">
       <c r="A301" s="12">
         <f t="shared" si="9"/>
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B301" s="13" t="s">
         <v>696</v>
@@ -12308,7 +12308,7 @@
     <row r="302">
       <c r="A302" s="12">
         <f t="shared" si="9"/>
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B302" s="13" t="s">
         <v>698</v>
@@ -12336,7 +12336,7 @@
     <row r="303">
       <c r="A303" s="12">
         <f t="shared" si="9"/>
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B303" s="13" t="s">
         <v>700</v>
@@ -12364,7 +12364,7 @@
     <row r="304">
       <c r="A304" s="12">
         <f t="shared" si="9"/>
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B304" s="13" t="s">
         <v>702</v>
@@ -12392,7 +12392,7 @@
     <row r="305">
       <c r="A305" s="12">
         <f t="shared" si="9"/>
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B305" s="13" t="s">
         <v>368</v>
@@ -12420,7 +12420,7 @@
     <row r="306">
       <c r="A306" s="12">
         <f t="shared" si="9"/>
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B306" s="13" t="s">
         <v>705</v>
@@ -12448,7 +12448,7 @@
     <row r="307">
       <c r="A307" s="12">
         <f t="shared" si="9"/>
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B307" s="13" t="s">
         <v>707</v>
@@ -12476,7 +12476,7 @@
     <row r="308">
       <c r="A308" s="12">
         <f t="shared" si="9"/>
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B308" s="13" t="s">
         <v>709</v>
@@ -12504,7 +12504,7 @@
     <row r="309">
       <c r="A309" s="12">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B309" s="13" t="s">
         <v>711</v>
@@ -12532,7 +12532,7 @@
     <row r="310">
       <c r="A310" s="12">
         <f t="shared" si="9"/>
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B310" s="13" t="s">
         <v>713</v>

</xml_diff>